<commit_message>
more calculations and cell additions
</commit_message>
<xml_diff>
--- a/Column Mappings.xlsx
+++ b/Column Mappings.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swanson/Projects/4CforChildren/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92606142-1E53-464D-B71B-315806FAAD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E7AA3D-E393-0B4E-A740-BB40290A9FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{512204E7-A817-684C-88F8-321F4B4C0825}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -461,10 +461,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE92296D-198E-A84C-B234-229B9CBE853F}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="108.83203125" defaultRowHeight="22" x14ac:dyDescent="0.3"/>

</xml_diff>